<commit_message>
Results removed shared words
</commit_message>
<xml_diff>
--- a/experiments/hybrid/train.0.001/2-gram-weights.xlsx
+++ b/experiments/hybrid/train.0.001/2-gram-weights.xlsx
@@ -456,423 +456,423 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.03007518796992481</v>
+        <v>0.03053435114503817</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>('video', 'game')</t>
+          <t>('zombie', 'planet')</t>
         </is>
       </c>
       <c r="B3" t="n">
         <v>3</v>
       </c>
       <c r="C3" t="n">
-        <v>0.02255639097744361</v>
+        <v>0.02290076335877863</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>('made', 'movie')</t>
+          <t>('someone', 'else')</t>
         </is>
       </c>
       <c r="B4" t="n">
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>0.02255639097744361</v>
+        <v>0.02290076335877863</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>('main', 'character')</t>
+          <t>('skeletor', 'attacks')</t>
         </is>
       </c>
       <c r="B5" t="n">
         <v>3</v>
       </c>
       <c r="C5" t="n">
-        <v>0.02255639097744361</v>
+        <v>0.02290076335877863</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>('film', 'making')</t>
+          <t>('way', 'adjl')</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>3</v>
       </c>
       <c r="C6" t="n">
-        <v>0.02255639097744361</v>
+        <v>0.02290076335877863</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>('music', 'videos')</t>
+          <t>('video', 'game')</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>3</v>
       </c>
       <c r="C7" t="n">
-        <v>0.02255639097744361</v>
+        <v>0.02290076335877863</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>('zombie', 'planet')</t>
+          <t>('music', 'videos')</t>
         </is>
       </c>
       <c r="B8" t="n">
         <v>3</v>
       </c>
       <c r="C8" t="n">
-        <v>0.02255639097744361</v>
+        <v>0.02290076335877863</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>('way', 'adjl')</t>
+          <t>('film', 'making')</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>3</v>
       </c>
       <c r="C9" t="n">
-        <v>0.02255639097744361</v>
+        <v>0.02290076335877863</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>('skeletor', 'attacks')</t>
+          <t>('main', 'character')</t>
         </is>
       </c>
       <c r="B10" t="n">
         <v>3</v>
       </c>
       <c r="C10" t="n">
-        <v>0.02255639097744361</v>
+        <v>0.02290076335877863</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>('even', 'though')</t>
+          <t>('made', 'movie')</t>
         </is>
       </c>
       <c r="B11" t="n">
         <v>3</v>
       </c>
       <c r="C11" t="n">
-        <v>0.02255639097744361</v>
+        <v>0.02290076335877863</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>('someone', 'else')</t>
+          <t>('adjl', 'like')</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C12" t="n">
-        <v>0.02255639097744361</v>
+        <v>0.01526717557251908</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>('macho', 'bs')</t>
+          <t>('title', 'cards')</t>
         </is>
       </c>
       <c r="B13" t="n">
         <v>2</v>
       </c>
       <c r="C13" t="n">
-        <v>0.01503759398496241</v>
+        <v>0.01526717557251908</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>('movie', 'least')</t>
+          <t>('became', 'increasingly')</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>2</v>
       </c>
       <c r="C14" t="n">
-        <v>0.01503759398496241</v>
+        <v>0.01526717557251908</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>('watching', 'movie')</t>
+          <t>('first', 'place')</t>
         </is>
       </c>
       <c r="B15" t="n">
         <v>2</v>
       </c>
       <c r="C15" t="n">
-        <v>0.01503759398496241</v>
+        <v>0.01526717557251908</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>('finished', 'watching')</t>
+          <t>('adjl', 'anime')</t>
         </is>
       </c>
       <c r="B16" t="n">
         <v>2</v>
       </c>
       <c r="C16" t="n">
-        <v>0.01503759398496241</v>
+        <v>0.01526717557251908</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>('bad', 'episode')</t>
+          <t>('military', 'macho')</t>
         </is>
       </c>
       <c r="B17" t="n">
         <v>2</v>
       </c>
       <c r="C17" t="n">
-        <v>0.01503759398496241</v>
+        <v>0.01526717557251908</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>('worth', 'time')</t>
+          <t>('quasi', 'military')</t>
         </is>
       </c>
       <c r="B18" t="n">
         <v>2</v>
       </c>
       <c r="C18" t="n">
-        <v>0.01503759398496241</v>
+        <v>0.01526717557251908</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>('pretty', 'much')</t>
+          <t>('movie', 'terrible')</t>
         </is>
       </c>
       <c r="B19" t="n">
         <v>2</v>
       </c>
       <c r="C19" t="n">
-        <v>0.01503759398496241</v>
+        <v>0.01526717557251908</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>('dream', 'oh')</t>
+          <t>('opening', 'scenes')</t>
         </is>
       </c>
       <c r="B20" t="n">
         <v>2</v>
       </c>
       <c r="C20" t="n">
-        <v>0.01503759398496241</v>
+        <v>0.01526717557251908</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>('oh', 'dream')</t>
+          <t>('dark', 'room')</t>
         </is>
       </c>
       <c r="B21" t="n">
         <v>2</v>
       </c>
       <c r="C21" t="n">
-        <v>0.01503759398496241</v>
+        <v>0.01526717557251908</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>('cliched', 'predictable')</t>
+          <t>('make', 'documentary')</t>
         </is>
       </c>
       <c r="B22" t="n">
         <v>2</v>
       </c>
       <c r="C22" t="n">
-        <v>0.01503759398496241</v>
+        <v>0.01526717557251908</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>('actors', 'actresses')</t>
+          <t>('low', 'budget')</t>
         </is>
       </c>
       <c r="B23" t="n">
         <v>2</v>
       </c>
       <c r="C23" t="n">
-        <v>0.01503759398496241</v>
+        <v>0.01526717557251908</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>('make', 'movie')</t>
+          <t>('ridiculously', 'bad')</t>
         </is>
       </c>
       <c r="B24" t="n">
         <v>2</v>
       </c>
       <c r="C24" t="n">
-        <v>0.01503759398496241</v>
+        <v>0.01526717557251908</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>('game', 'first')</t>
+          <t>('van', 'diem')</t>
         </is>
       </c>
       <c r="B25" t="n">
         <v>2</v>
       </c>
       <c r="C25" t="n">
-        <v>0.01503759398496241</v>
+        <v>0.01526717557251908</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>('version', 'even')</t>
+          <t>('film', 'could')</t>
         </is>
       </c>
       <c r="B26" t="n">
         <v>2</v>
       </c>
       <c r="C26" t="n">
-        <v>0.01503759398496241</v>
+        <v>0.01526717557251908</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>('selma', 'blair')</t>
+          <t>('law', 'order')</t>
         </is>
       </c>
       <c r="B27" t="n">
         <v>2</v>
       </c>
       <c r="C27" t="n">
-        <v>0.01503759398496241</v>
+        <v>0.01526717557251908</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>('various', 'things')</t>
+          <t>('worst', 'part')</t>
         </is>
       </c>
       <c r="B28" t="n">
         <v>2</v>
       </c>
       <c r="C28" t="n">
-        <v>0.01503759398496241</v>
+        <v>0.01526717557251908</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>('movie', 'like')</t>
+          <t>('behind', 'tree')</t>
         </is>
       </c>
       <c r="B29" t="n">
         <v>2</v>
       </c>
       <c r="C29" t="n">
-        <v>0.01503759398496241</v>
+        <v>0.01526717557251908</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>('utility', 'worker')</t>
+          <t>('version', 'csi')</t>
         </is>
       </c>
       <c r="B30" t="n">
         <v>2</v>
       </c>
       <c r="C30" t="n">
-        <v>0.01503759398496241</v>
+        <v>0.01526717557251908</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>('home', 'version')</t>
+          <t>('kill', 'later')</t>
         </is>
       </c>
       <c r="B31" t="n">
         <v>2</v>
       </c>
       <c r="C31" t="n">
-        <v>0.01503759398496241</v>
+        <v>0.01526717557251908</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>('mirror', 'mirror')</t>
+          <t>('could', 'spent')</t>
         </is>
       </c>
       <c r="B32" t="n">
         <v>2</v>
       </c>
       <c r="C32" t="n">
-        <v>0.01503759398496241</v>
+        <v>0.01526717557251908</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>('part', 'movie')</t>
+          <t>('money', 'good')</t>
         </is>
       </c>
       <c r="B33" t="n">
         <v>2</v>
       </c>
       <c r="C33" t="n">
-        <v>0.01503759398496241</v>
+        <v>0.01526717557251908</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>('perhaps', 'better')</t>
+          <t>('special', 'effects')</t>
         </is>
       </c>
       <c r="B34" t="n">
         <v>2</v>
       </c>
       <c r="C34" t="n">
-        <v>0.01503759398496241</v>
+        <v>0.01526717557251908</v>
       </c>
     </row>
     <row r="35">
@@ -885,397 +885,397 @@
         <v>2</v>
       </c>
       <c r="C35" t="n">
-        <v>0.01503759398496241</v>
+        <v>0.01526717557251908</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>('law', 'order')</t>
+          <t>('actors', 'actresses')</t>
         </is>
       </c>
       <c r="B36" t="n">
         <v>2</v>
       </c>
       <c r="C36" t="n">
-        <v>0.01503759398496241</v>
+        <v>0.01526717557251908</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>('money', 'good')</t>
+          <t>('macho', 'bs')</t>
         </is>
       </c>
       <c r="B37" t="n">
         <v>2</v>
       </c>
       <c r="C37" t="n">
-        <v>0.01503759398496241</v>
+        <v>0.01526717557251908</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>('title', 'cards')</t>
+          <t>('perhaps', 'better')</t>
         </is>
       </c>
       <c r="B38" t="n">
         <v>2</v>
       </c>
       <c r="C38" t="n">
-        <v>0.01503759398496241</v>
+        <v>0.01526717557251908</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>('became', 'increasingly')</t>
+          <t>('movie', 'least')</t>
         </is>
       </c>
       <c r="B39" t="n">
         <v>2</v>
       </c>
       <c r="C39" t="n">
-        <v>0.01503759398496241</v>
+        <v>0.01526717557251908</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>('first', 'place')</t>
+          <t>('watching', 'movie')</t>
         </is>
       </c>
       <c r="B40" t="n">
         <v>2</v>
       </c>
       <c r="C40" t="n">
-        <v>0.01503759398496241</v>
+        <v>0.01526717557251908</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>('adjl', 'anime')</t>
+          <t>('bad', 'episode')</t>
         </is>
       </c>
       <c r="B41" t="n">
         <v>2</v>
       </c>
       <c r="C41" t="n">
-        <v>0.01503759398496241</v>
+        <v>0.01526717557251908</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>('military', 'macho')</t>
+          <t>('worth', 'time')</t>
         </is>
       </c>
       <c r="B42" t="n">
         <v>2</v>
       </c>
       <c r="C42" t="n">
-        <v>0.01503759398496241</v>
+        <v>0.01526717557251908</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>('quasi', 'military')</t>
+          <t>('pretty', 'much')</t>
         </is>
       </c>
       <c r="B43" t="n">
         <v>2</v>
       </c>
       <c r="C43" t="n">
-        <v>0.01503759398496241</v>
+        <v>0.01526717557251908</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>('movie', 'terrible')</t>
+          <t>('dream', 'oh')</t>
         </is>
       </c>
       <c r="B44" t="n">
         <v>2</v>
       </c>
       <c r="C44" t="n">
-        <v>0.01503759398496241</v>
+        <v>0.01526717557251908</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>('opening', 'scenes')</t>
+          <t>('oh', 'dream')</t>
         </is>
       </c>
       <c r="B45" t="n">
         <v>2</v>
       </c>
       <c r="C45" t="n">
-        <v>0.01503759398496241</v>
+        <v>0.01526717557251908</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>('dark', 'room')</t>
+          <t>('cliched', 'predictable')</t>
         </is>
       </c>
       <c r="B46" t="n">
         <v>2</v>
       </c>
       <c r="C46" t="n">
-        <v>0.01503759398496241</v>
+        <v>0.01526717557251908</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>('adjl', 'like')</t>
+          <t>('finished', 'watching')</t>
         </is>
       </c>
       <c r="B47" t="n">
         <v>2</v>
       </c>
       <c r="C47" t="n">
-        <v>0.01503759398496241</v>
+        <v>0.01526717557251908</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>('special', 'effects')</t>
+          <t>('home', 'version')</t>
         </is>
       </c>
       <c r="B48" t="n">
         <v>2</v>
       </c>
       <c r="C48" t="n">
-        <v>0.01503759398496241</v>
+        <v>0.01526717557251908</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>('low', 'budget')</t>
+          <t>('movie', 'like')</t>
         </is>
       </c>
       <c r="B49" t="n">
         <v>2</v>
       </c>
       <c r="C49" t="n">
-        <v>0.01503759398496241</v>
+        <v>0.01526717557251908</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>('ridiculously', 'bad')</t>
+          <t>('mirror', 'mirror')</t>
         </is>
       </c>
       <c r="B50" t="n">
         <v>2</v>
       </c>
       <c r="C50" t="n">
-        <v>0.01503759398496241</v>
+        <v>0.01526717557251908</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>('van', 'diem')</t>
+          <t>('make', 'movie')</t>
         </is>
       </c>
       <c r="B51" t="n">
         <v>2</v>
       </c>
       <c r="C51" t="n">
-        <v>0.01503759398496241</v>
+        <v>0.01526717557251908</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>('film', 'could')</t>
+          <t>('utility', 'worker')</t>
         </is>
       </c>
       <c r="B52" t="n">
         <v>2</v>
       </c>
       <c r="C52" t="n">
-        <v>0.01503759398496241</v>
+        <v>0.01526717557251908</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>('make', 'documentary')</t>
+          <t>('part', 'movie')</t>
         </is>
       </c>
       <c r="B53" t="n">
         <v>2</v>
       </c>
       <c r="C53" t="n">
-        <v>0.01503759398496241</v>
+        <v>0.01526717557251908</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>('worst', 'part')</t>
+          <t>('various', 'things')</t>
         </is>
       </c>
       <c r="B54" t="n">
         <v>2</v>
       </c>
       <c r="C54" t="n">
-        <v>0.01503759398496241</v>
+        <v>0.01526717557251908</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>('behind', 'tree')</t>
+          <t>('selma', 'blair')</t>
         </is>
       </c>
       <c r="B55" t="n">
         <v>2</v>
       </c>
       <c r="C55" t="n">
-        <v>0.01503759398496241</v>
+        <v>0.01526717557251908</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>('version', 'csi')</t>
+          <t>('version', 'even')</t>
         </is>
       </c>
       <c r="B56" t="n">
         <v>2</v>
       </c>
       <c r="C56" t="n">
-        <v>0.01503759398496241</v>
+        <v>0.01526717557251908</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
         <is>
-          <t>('kill', 'later')</t>
+          <t>('game', 'first')</t>
         </is>
       </c>
       <c r="B57" t="n">
         <v>2</v>
       </c>
       <c r="C57" t="n">
-        <v>0.01503759398496241</v>
+        <v>0.01526717557251908</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
         <is>
-          <t>('could', 'spent')</t>
+          <t>('reasons', 'one')</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C58" t="n">
-        <v>0.01503759398496241</v>
+        <v>0.007633587786259542</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
         <is>
-          <t>('jumping', 'top')</t>
+          <t>('compromise', 'quality')</t>
         </is>
       </c>
       <c r="B59" t="n">
         <v>1</v>
       </c>
       <c r="C59" t="n">
-        <v>0.007518796992481203</v>
+        <v>0.007633587786259542</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
         <is>
-          <t>('bank', 'robber')</t>
+          <t>('without', 'reasons')</t>
         </is>
       </c>
       <c r="B60" t="n">
         <v>1</v>
       </c>
       <c r="C60" t="n">
-        <v>0.007518796992481203</v>
+        <v>0.007633587786259542</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
         <is>
-          <t>('max', 'beesley')</t>
+          <t>('making', 'movie')</t>
         </is>
       </c>
       <c r="B61" t="n">
         <v>1</v>
       </c>
       <c r="C61" t="n">
-        <v>0.007518796992481203</v>
+        <v>0.007633587786259542</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
         <is>
-          <t>('top', 'office')</t>
+          <t>('lauren', 'adams')</t>
         </is>
       </c>
       <c r="B62" t="n">
         <v>1</v>
       </c>
       <c r="C62" t="n">
-        <v>0.007518796992481203</v>
+        <v>0.007633587786259542</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
         <is>
-          <t>('office', 'building')</t>
+          <t>('secure', 'good')</t>
         </is>
       </c>
       <c r="B63" t="n">
         <v>1</v>
       </c>
       <c r="C63" t="n">
-        <v>0.007518796992481203</v>
+        <v>0.007633587786259542</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
         <is>
-          <t>('building', 'protects')</t>
+          <t>('finance', 'film')</t>
         </is>
       </c>
       <c r="B64" t="n">
         <v>1</v>
       </c>
       <c r="C64" t="n">
-        <v>0.007518796992481203</v>
+        <v>0.007633587786259542</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
         <is>
-          <t>('protects', 'bank')</t>
+          <t>('falls', 'flat')</t>
         </is>
       </c>
       <c r="B65" t="n">
         <v>1</v>
       </c>
       <c r="C65" t="n">
-        <v>0.007518796992481203</v>
+        <v>0.007633587786259542</v>
       </c>
     </row>
   </sheetData>
@@ -1319,59 +1319,59 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>0.05714285714285714</v>
+        <v>0.0576923076923077</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>('english', 'patient')</t>
+          <t>('jude', 'law')</t>
         </is>
       </c>
       <c r="B3" t="n">
         <v>4</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0380952380952381</v>
+        <v>0.03846153846153846</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>('jude', 'law')</t>
+          <t>('cold', 'mountain')</t>
         </is>
       </c>
       <c r="B4" t="n">
         <v>4</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0380952380952381</v>
+        <v>0.03846153846153846</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>('cold', 'mountain')</t>
+          <t>('nicole', 'kidman')</t>
         </is>
       </c>
       <c r="B5" t="n">
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0380952380952381</v>
+        <v>0.03846153846153846</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>('nicole', 'kidman')</t>
+          <t>('english', 'patient')</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0380952380952381</v>
+        <v>0.03846153846153846</v>
       </c>
     </row>
     <row r="7">
@@ -1384,761 +1384,761 @@
         <v>3</v>
       </c>
       <c r="C7" t="n">
-        <v>0.02857142857142857</v>
+        <v>0.02884615384615385</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>('looks', 'like')</t>
+          <t>('film', 'work')</t>
         </is>
       </c>
       <c r="B8" t="n">
         <v>2</v>
       </c>
       <c r="C8" t="n">
-        <v>0.01904761904761905</v>
+        <v>0.01923076923076923</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>('films', 'ever')</t>
+          <t>('oscar', 'winner')</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>2</v>
       </c>
       <c r="C9" t="n">
-        <v>0.01904761904761905</v>
+        <v>0.01923076923076923</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>('even', 'though')</t>
+          <t>('film', 'seen')</t>
         </is>
       </c>
       <c r="B10" t="n">
         <v>2</v>
       </c>
       <c r="C10" t="n">
-        <v>0.01904761904761905</v>
+        <v>0.01923076923076923</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>('movie', 'would')</t>
+          <t>('love', 'affair')</t>
         </is>
       </c>
       <c r="B11" t="n">
         <v>2</v>
       </c>
       <c r="C11" t="n">
-        <v>0.01904761904761905</v>
+        <v>0.01923076923076923</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>('alan', 'rickman')</t>
+          <t>('battleship', 'potemkin')</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>2</v>
       </c>
       <c r="C12" t="n">
-        <v>0.01904761904761905</v>
+        <v>0.01923076923076923</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>('mick', 'molloy')</t>
+          <t>('renee', 'zellwegger')</t>
         </is>
       </c>
       <c r="B13" t="n">
         <v>2</v>
       </c>
       <c r="C13" t="n">
-        <v>0.01904761904761905</v>
+        <v>0.01923076923076923</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>('new', 'york')</t>
+          <t>('work', 'art')</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>2</v>
       </c>
       <c r="C14" t="n">
-        <v>0.01904761904761905</v>
+        <v>0.01923076923076923</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>('civil', 'war')</t>
+          <t>('believe', 'movie')</t>
         </is>
       </c>
       <c r="B15" t="n">
         <v>2</v>
       </c>
       <c r="C15" t="n">
-        <v>0.01904761904761905</v>
+        <v>0.01923076923076923</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>('one', 'best')</t>
+          <t>('ever', 'seen')</t>
         </is>
       </c>
       <c r="B16" t="n">
         <v>2</v>
       </c>
       <c r="C16" t="n">
-        <v>0.01904761904761905</v>
+        <v>0.01923076923076923</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>('anthony', 'minghella')</t>
+          <t>('film', 'everyone')</t>
         </is>
       </c>
       <c r="B17" t="n">
         <v>2</v>
       </c>
       <c r="C17" t="n">
-        <v>0.01904761904761905</v>
+        <v>0.01923076923076923</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>('director', 'anthony')</t>
+          <t>('holly', 'would')</t>
         </is>
       </c>
       <c r="B18" t="n">
         <v>2</v>
       </c>
       <c r="C18" t="n">
-        <v>0.01904761904761905</v>
+        <v>0.01923076923076923</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>('film', 'work')</t>
+          <t>('director', 'anthony')</t>
         </is>
       </c>
       <c r="B19" t="n">
         <v>2</v>
       </c>
       <c r="C19" t="n">
-        <v>0.01904761904761905</v>
+        <v>0.01923076923076923</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>('film', 'everyone')</t>
+          <t>('one', 'best')</t>
         </is>
       </c>
       <c r="B20" t="n">
         <v>2</v>
       </c>
       <c r="C20" t="n">
-        <v>0.01904761904761905</v>
+        <v>0.01923076923076923</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>('ever', 'seen')</t>
+          <t>('civil', 'war')</t>
         </is>
       </c>
       <c r="B21" t="n">
         <v>2</v>
       </c>
       <c r="C21" t="n">
-        <v>0.01904761904761905</v>
+        <v>0.01923076923076923</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>('believe', 'movie')</t>
+          <t>('new', 'york')</t>
         </is>
       </c>
       <c r="B22" t="n">
         <v>2</v>
       </c>
       <c r="C22" t="n">
-        <v>0.01904761904761905</v>
+        <v>0.01923076923076923</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>('work', 'art')</t>
+          <t>('mick', 'molloy')</t>
         </is>
       </c>
       <c r="B23" t="n">
         <v>2</v>
       </c>
       <c r="C23" t="n">
-        <v>0.01904761904761905</v>
+        <v>0.01923076923076923</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>('renee', 'zellwegger')</t>
+          <t>('alan', 'rickman')</t>
         </is>
       </c>
       <c r="B24" t="n">
         <v>2</v>
       </c>
       <c r="C24" t="n">
-        <v>0.01904761904761905</v>
+        <v>0.01923076923076923</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>('battleship', 'potemkin')</t>
+          <t>('movie', 'would')</t>
         </is>
       </c>
       <c r="B25" t="n">
         <v>2</v>
       </c>
       <c r="C25" t="n">
-        <v>0.01904761904761905</v>
+        <v>0.01923076923076923</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>('love', 'affair')</t>
+          <t>('films', 'ever')</t>
         </is>
       </c>
       <c r="B26" t="n">
         <v>2</v>
       </c>
       <c r="C26" t="n">
-        <v>0.01904761904761905</v>
+        <v>0.01923076923076923</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>('film', 'seen')</t>
+          <t>('looks', 'like')</t>
         </is>
       </c>
       <c r="B27" t="n">
         <v>2</v>
       </c>
       <c r="C27" t="n">
-        <v>0.01904761904761905</v>
+        <v>0.01923076923076923</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>('holly', 'would')</t>
+          <t>('anthony', 'minghella')</t>
         </is>
       </c>
       <c r="B28" t="n">
         <v>2</v>
       </c>
       <c r="C28" t="n">
-        <v>0.01904761904761905</v>
+        <v>0.01923076923076923</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>('oscar', 'winner')</t>
+          <t>('existence', 'tale')</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C29" t="n">
-        <v>0.01904761904761905</v>
+        <v>0.009615384615384616</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>('treason', 'tantalizing')</t>
+          <t>('special', 'story')</t>
         </is>
       </c>
       <c r="B30" t="n">
         <v>1</v>
       </c>
       <c r="C30" t="n">
-        <v>0.009523809523809525</v>
+        <v>0.009615384615384616</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>('characters', 'married')</t>
+          <t>('story', 'ambiguity')</t>
         </is>
       </c>
       <c r="B31" t="n">
         <v>1</v>
       </c>
       <c r="C31" t="n">
-        <v>0.009523809523809525</v>
+        <v>0.009615384615384616</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>('sexual', 'energy')</t>
+          <t>('ambiguity', 'existence')</t>
         </is>
       </c>
       <c r="B32" t="n">
         <v>1</v>
       </c>
       <c r="C32" t="n">
-        <v>0.009523809523809525</v>
+        <v>0.009615384615384616</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>('nightmare', 'always')</t>
+          <t>('innocence', 'error')</t>
         </is>
       </c>
       <c r="B33" t="n">
         <v>1</v>
       </c>
       <c r="C33" t="n">
-        <v>0.009523809523809525</v>
+        <v>0.009615384615384616</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>('always', 'seems')</t>
+          <t>('tale', 'kafka')</t>
         </is>
       </c>
       <c r="B34" t="n">
         <v>1</v>
       </c>
       <c r="C34" t="n">
-        <v>0.009523809523809525</v>
+        <v>0.009615384615384616</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>('seems', 'far')</t>
+          <t>('kafka', 'style')</t>
         </is>
       </c>
       <c r="B35" t="n">
         <v>1</v>
       </c>
       <c r="C35" t="n">
-        <v>0.009523809523809525</v>
+        <v>0.009615384615384616</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>('far', 'away')</t>
+          <t>('surviving', 'perpetual')</t>
         </is>
       </c>
       <c r="B36" t="n">
         <v>1</v>
       </c>
       <c r="C36" t="n">
-        <v>0.009523809523809525</v>
+        <v>0.009615384615384616</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>('away', 'dark')</t>
+          <t>('love', 'love')</t>
         </is>
       </c>
       <c r="B37" t="n">
         <v>1</v>
       </c>
       <c r="C37" t="n">
-        <v>0.009523809523809525</v>
+        <v>0.009615384615384616</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>('dark', 'habour')</t>
+          <t>('doubtlessly', 'special')</t>
         </is>
       </c>
       <c r="B38" t="n">
         <v>1</v>
       </c>
       <c r="C38" t="n">
-        <v>0.009523809523809525</v>
+        <v>0.009615384615384616</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>('habour', 'characters')</t>
+          <t>('piece', 'subtle')</t>
         </is>
       </c>
       <c r="B39" t="n">
         <v>1</v>
       </c>
       <c r="C39" t="n">
-        <v>0.009523809523809525</v>
+        <v>0.009615384615384616</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>('hunter', 'vagabond')</t>
+          <t>('masterpiece', 'doubtlessly')</t>
         </is>
       </c>
       <c r="B40" t="n">
         <v>1</v>
       </c>
       <c r="C40" t="n">
-        <v>0.009523809523809525</v>
+        <v>0.009615384615384616</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>('married', 'couple')</t>
+          <t>('maybe', 'masterpiece')</t>
         </is>
       </c>
       <c r="B41" t="n">
         <v>1</v>
       </c>
       <c r="C41" t="n">
-        <v>0.009523809523809525</v>
+        <v>0.009615384615384616</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>('energy', 'treason')</t>
+          <t>('perpetual', 'strange')</t>
         </is>
       </c>
       <c r="B42" t="n">
         <v>1</v>
       </c>
       <c r="C42" t="n">
-        <v>0.009523809523809525</v>
+        <v>0.009615384615384616</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>('couple', 'alan')</t>
+          <t>('art', 'maybe')</t>
         </is>
       </c>
       <c r="B43" t="n">
         <v>1</v>
       </c>
       <c r="C43" t="n">
-        <v>0.009523809523809525</v>
+        <v>0.009615384615384616</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>('polly', 'hunter')</t>
+          <t>('well', 'done')</t>
         </is>
       </c>
       <c r="B44" t="n">
         <v>1</v>
       </c>
       <c r="C44" t="n">
-        <v>0.009523809523809525</v>
+        <v>0.009615384615384616</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>('vagabond', 'norman')</t>
+          <t>('movie', 'well')</t>
         </is>
       </c>
       <c r="B45" t="n">
         <v>1</v>
       </c>
       <c r="C45" t="n">
-        <v>0.009523809523809525</v>
+        <v>0.009615384615384616</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>('norman', 'reedus')</t>
+          <t>('time', 'movie')</t>
         </is>
       </c>
       <c r="B46" t="n">
         <v>1</v>
       </c>
       <c r="C46" t="n">
-        <v>0.009523809523809525</v>
+        <v>0.009615384615384616</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>('reedus', 'slipping')</t>
+          <t>('prime', 'time')</t>
         </is>
       </c>
       <c r="B47" t="n">
         <v>1</v>
       </c>
       <c r="C47" t="n">
-        <v>0.009523809523809525</v>
+        <v>0.009615384615384616</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>('slipping', 'game')</t>
+          <t>('typical', 'prime')</t>
         </is>
       </c>
       <c r="B48" t="n">
         <v>1</v>
       </c>
       <c r="C48" t="n">
-        <v>0.009523809523809525</v>
+        <v>0.009615384615384616</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>('game', 'full')</t>
+          <t>('conclusion', 'typical')</t>
         </is>
       </c>
       <c r="B49" t="n">
         <v>1</v>
       </c>
       <c r="C49" t="n">
-        <v>0.009523809523809525</v>
+        <v>0.009615384615384616</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>('full', 'hidden')</t>
+          <t>('love', 'movie')</t>
         </is>
       </c>
       <c r="B50" t="n">
         <v>1</v>
       </c>
       <c r="C50" t="n">
-        <v>0.009523809523809525</v>
+        <v>0.009615384615384616</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>('using', 'brain')</t>
+          <t>('sin', 'frailty')</t>
         </is>
       </c>
       <c r="B51" t="n">
         <v>1</v>
       </c>
       <c r="C51" t="n">
-        <v>0.009523809523809525</v>
+        <v>0.009615384615384616</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>('rickman', 'course')</t>
+          <t>('ways', 'leopold')</t>
         </is>
       </c>
       <c r="B52" t="n">
         <v>1</v>
       </c>
       <c r="C52" t="n">
-        <v>0.009523809523809525</v>
+        <v>0.009615384615384616</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>('good', 'acting')</t>
+          <t>('world', 'life')</t>
         </is>
       </c>
       <c r="B53" t="n">
         <v>1</v>
       </c>
       <c r="C53" t="n">
-        <v>0.009523809523809525</v>
+        <v>0.009615384615384616</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>('unconventionality', 'alan')</t>
+          <t>('leopold', 'kessle')</t>
         </is>
       </c>
       <c r="B54" t="n">
         <v>1</v>
       </c>
       <c r="C54" t="n">
-        <v>0.009523809523809525</v>
+        <v>0.009615384615384616</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>('rickman', 'polly')</t>
+          <t>('peace', 'business')</t>
         </is>
       </c>
       <c r="B55" t="n">
         <v>1</v>
       </c>
       <c r="C55" t="n">
-        <v>0.009523809523809525</v>
+        <v>0.009615384615384616</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>('europa', 'symbol')</t>
+          <t>('search', 'truth')</t>
         </is>
       </c>
       <c r="B56" t="n">
         <v>1</v>
       </c>
       <c r="C56" t="n">
-        <v>0.009523809523809525</v>
+        <v>0.009615384615384616</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
         <is>
-          <t>('ambiguous', 'woman')</t>
+          <t>('money', 'save')</t>
         </is>
       </c>
       <c r="B57" t="n">
         <v>1</v>
       </c>
       <c r="C57" t="n">
-        <v>0.009523809523809525</v>
+        <v>0.009615384615384616</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
         <is>
-          <t>('breaks', 'increase')</t>
+          <t>('couple', 'dollars')</t>
         </is>
       </c>
       <c r="B58" t="n">
         <v>1</v>
       </c>
       <c r="C58" t="n">
-        <v>0.009523809523809525</v>
+        <v>0.009615384615384616</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
         <is>
-          <t>('increase', 'tensions')</t>
+          <t>('earlier', 'work')</t>
         </is>
       </c>
       <c r="B59" t="n">
         <v>1</v>
       </c>
       <c r="C59" t="n">
-        <v>0.009523809523809525</v>
+        <v>0.009615384615384616</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
         <is>
-          <t>('tensions', 'give')</t>
+          <t>('images', 'trial')</t>
         </is>
       </c>
       <c r="B60" t="n">
         <v>1</v>
       </c>
       <c r="C60" t="n">
-        <v>0.009523809523809525</v>
+        <v>0.009615384615384616</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
         <is>
-          <t>('give', 'much')</t>
+          <t>('k', 'images')</t>
         </is>
       </c>
       <c r="B61" t="n">
         <v>1</v>
       </c>
       <c r="C61" t="n">
-        <v>0.009523809523809525</v>
+        <v>0.009615384615384616</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
         <is>
-          <t>('much', 'space')</t>
+          <t>('joseph', 'k')</t>
         </is>
       </c>
       <c r="B62" t="n">
         <v>1</v>
       </c>
       <c r="C62" t="n">
-        <v>0.009523809523809525</v>
+        <v>0.009615384615384616</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
         <is>
-          <t>('space', 'interpretations')</t>
+          <t>('another', 'joseph')</t>
         </is>
       </c>
       <c r="B63" t="n">
         <v>1</v>
       </c>
       <c r="C63" t="n">
-        <v>0.009523809523809525</v>
+        <v>0.009615384615384616</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
         <is>
-          <t>('interpretations', 'good')</t>
+          <t>('kessle', 'another')</t>
         </is>
       </c>
       <c r="B64" t="n">
         <v>1</v>
       </c>
       <c r="C64" t="n">
-        <v>0.009523809523809525</v>
+        <v>0.009615384615384616</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
         <is>
-          <t>('acting', 'story')</t>
+          <t>('victory', 'surviving')</t>
         </is>
       </c>
       <c r="B65" t="n">
         <v>1</v>
       </c>
       <c r="C65" t="n">
-        <v>0.009523809523809525</v>
+        <v>0.009615384615384616</v>
       </c>
     </row>
   </sheetData>

</xml_diff>